<commit_message>
Strategie 5 toegevoegd (8 in word doc)
</commit_message>
<xml_diff>
--- a/Logboek.xlsx
+++ b/Logboek.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>Taak</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>4u</t>
+  </si>
+  <si>
+    <t>Latex document aanpassen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulatie gegevens nakijken + verbeteren </t>
+  </si>
+  <si>
+    <t>1u</t>
   </si>
 </sst>
 </file>
@@ -160,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -169,6 +178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -452,7 +462,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -717,22 +727,38 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
+      <c r="A15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="8">
+        <v>42105</v>
+      </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="E15" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="6">
+        <v>42106</v>
+      </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="E16" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>

</xml_diff>